<commit_message>
Added codebase for Pandas Visualization
</commit_message>
<xml_diff>
--- a/car_data.xlsx
+++ b/car_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd21c5a53fb2ce41/Documents/Desktop/practice/Interview_prep_2024/github_repositories/python_coding/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_2FD355EDA9CC2DA71017B6EE0219589AD511DF74" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{888003DD-F626-46FA-8979-161C269AD0B9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -83,12 +89,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -102,6 +102,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,14 +133,23 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -142,6 +158,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -466,121 +490,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>174390</v>
       </c>
       <c r="C2" s="3">
         <v>42625</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>3.5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>75625</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>119780</v>
       </c>
       <c r="C3" s="3">
         <v>43675</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>4.5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>45400</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>97400</v>
       </c>
       <c r="C4" s="3">
         <v>40619</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>25000</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>71432</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>125000</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>2006</v>
       </c>
     </row>

</xml_diff>